<commit_message>
fixed bug where _FIXED_ columns weren't being removed. Added R:Theme
</commit_message>
<xml_diff>
--- a/system_overrides.xlsx
+++ b/system_overrides.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="76">
   <si>
     <t xml:space="preserve">Rules are processed in order by the finance app</t>
   </si>
@@ -188,6 +188,18 @@
   </si>
   <si>
     <t xml:space="preserve">Ticker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$theme=(.*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R:Theme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${theme}</t>
   </si>
   <si>
     <t xml:space="preserve">$=Capex.*</t>
@@ -351,13 +363,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ55"/>
+  <dimension ref="A1:AMJ57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A57" activeCellId="0" sqref="A57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A59" activeCellId="0" sqref="A59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.41"/>
@@ -678,80 +690,80 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="C38" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C39" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39" s="0" t="s">
+      <c r="D38" s="0" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>24</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B44" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C42" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>24</v>
+      <c r="C44" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -759,16 +771,13 @@
         <v>19</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="E47" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -776,45 +785,48 @@
         <v>19</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>40</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E49" s="1"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E50" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>67</v>
+      <c r="B51" s="0" t="s">
+        <v>69</v>
       </c>
       <c r="C51" s="0" t="s">
         <v>40</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>41</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E52" s="1"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>19</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>40</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -822,13 +834,27 @@
         <v>19</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>40</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>